<commit_message>
Definitive solution of "Access-Control-Allow-*" headers in the SiteHandlerOptions for Mozilla CORS.
</commit_message>
<xml_diff>
--- a/Documentation/AllConfigParameters.xlsx
+++ b/Documentation/AllConfigParameters.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Marlin\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381F5EA5-08F7-4F80-9E8F-F70CB457C48F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Blad1!$A$1:$M$85</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -404,7 +408,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -475,8 +479,36 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{4D6D20B4-078F-402C-B8EF-5C73F3113A00}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -784,14 +816,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="E67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A66" sqref="A66"/>
+      <selection pane="bottomRight" sqref="A1:M85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4012,7 +4047,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="54" fitToHeight="2" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>